<commit_message>
Commit ke sebelas dari jimmy
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>SCRUMMASTER</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Karena lupa screenshot terpaksa saya pindah lagi ke awal-awal</t>
+  </si>
+  <si>
+    <t>dari Jimmy Yappeter ( 13.111.0461 )</t>
+  </si>
+  <si>
+    <t>tgl 05 Juni 2015</t>
   </si>
 </sst>
 </file>
@@ -108,10 +114,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -156,6 +162,49 @@
         <a:xfrm>
           <a:off x="619126" y="613684"/>
           <a:ext cx="7985669" cy="4761138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>68525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="SS.PNG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619126" y="571501"/>
+          <a:ext cx="6953250" cy="3688024"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -464,58 +513,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -559,14 +608,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>